<commit_message>
Use for ES6 install Babel and add 'XLSX' module, parsed table Code luffing & fix
</commit_message>
<xml_diff>
--- a/LTM_1500-8.1.xlsx
+++ b/LTM_1500-8.1.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="465" windowWidth="21600" windowHeight="17805" tabRatio="695" firstSheet="15" activeTab="23"/>
+    <workbookView xWindow="16800" yWindow="465" windowWidth="21600" windowHeight="17805" tabRatio="695" firstSheet="16" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="T_165t_TAB221355" sheetId="2" r:id="rId1"/>
-    <sheet name="T_135t" sheetId="3" r:id="rId2"/>
-    <sheet name="T_105t" sheetId="4" r:id="rId3"/>
+    <sheet name="T_135t_TAB221355" sheetId="3" r:id="rId2"/>
+    <sheet name="T_105t_TAB221355" sheetId="4" r:id="rId3"/>
     <sheet name="T_90t_TAB221363" sheetId="5" r:id="rId4"/>
     <sheet name="T_75t_TAB221364" sheetId="6" r:id="rId5"/>
-    <sheet name="TY3_165t_TAB221364" sheetId="7" r:id="rId6"/>
-    <sheet name="TY3_135t_TAB221364" sheetId="8" r:id="rId7"/>
-    <sheet name="TF_135t_TAB221624" sheetId="9" r:id="rId8"/>
-    <sheet name="TF_135t_TAB221632" sheetId="10" r:id="rId9"/>
+    <sheet name="TY3_165t_TAB223026" sheetId="7" r:id="rId6"/>
+    <sheet name="TY3_135t_TAB223027" sheetId="8" r:id="rId7"/>
+    <sheet name="TF_135t_TAB221624.1" sheetId="9" r:id="rId8"/>
+    <sheet name="TF_135t_TAB221624.2" sheetId="10" r:id="rId9"/>
     <sheet name="TF_135t_TAB221640" sheetId="11" r:id="rId10"/>
     <sheet name="TF_135t_TAB221640.1" sheetId="13" r:id="rId11"/>
     <sheet name="TF_135t_TAB221640.2" sheetId="12" r:id="rId12"/>
@@ -36,6 +36,7 @@
     <sheet name="TN_165t_TAB231132.3" sheetId="25" r:id="rId22"/>
     <sheet name="TN_165t_TAB231142.1" sheetId="26" r:id="rId23"/>
     <sheet name="TN_165t_TAB231142.2" sheetId="27" r:id="rId24"/>
+    <sheet name="TNZF_135t_TAB231265" sheetId="29" r:id="rId25"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="25">
   <si>
     <t>TAB 221355</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -116,10 +117,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TAB 221364</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>러핑길이</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -141,6 +138,18 @@
   </si>
   <si>
     <t>TAB 231142</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAB 223026</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAB 223027</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TAB 231265</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1555,7 +1564,7 @@
   <dimension ref="A1:AC63"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:AA5"/>
+      <selection activeCell="AA54" sqref="A1:AA54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25"/>
@@ -14405,7 +14414,7 @@
   <dimension ref="A1:AA63"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="V1" sqref="V1:V1048576"/>
+      <selection activeCell="AA54" sqref="A1:AA54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25"/>
@@ -17659,7 +17668,7 @@
   <dimension ref="A1:W48"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W48" sqref="W48"/>
+      <selection activeCell="Y13" sqref="Y13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -17883,7 +17892,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>21</v>
@@ -17954,7 +17963,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="13">
         <v>83</v>
@@ -20013,7 +20022,7 @@
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
       <c r="W48" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -20251,7 +20260,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>21</v>
@@ -20322,7 +20331,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="13">
         <v>83</v>
@@ -22353,7 +22362,7 @@
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
       <c r="W48" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -22609,7 +22618,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>21</v>
@@ -22686,7 +22695,7 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="13">
         <v>83</v>
@@ -24406,7 +24415,7 @@
       <c r="W41" s="6"/>
       <c r="X41" s="6"/>
       <c r="Y41" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -25440,7 +25449,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>21</v>
@@ -25511,7 +25520,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="13">
         <v>75</v>
@@ -27410,7 +27419,7 @@
       <c r="U48" s="6"/>
       <c r="V48" s="6"/>
       <c r="W48" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -27648,7 +27657,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>21</v>
@@ -27719,7 +27728,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="13">
         <v>75</v>
@@ -29467,7 +29476,7 @@
       <c r="U45" s="6"/>
       <c r="V45" s="6"/>
       <c r="W45" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -29642,7 +29651,7 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>21</v>
@@ -29692,7 +29701,7 @@
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="13">
         <v>75</v>
@@ -30403,7 +30412,7 @@
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -30641,7 +30650,7 @@
     </row>
     <row r="4" spans="1:23">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>21</v>
@@ -30712,7 +30721,7 @@
     </row>
     <row r="5" spans="1:23">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="13">
         <v>67</v>
@@ -32399,7 +32408,7 @@
       <c r="U46" s="6"/>
       <c r="V46" s="6"/>
       <c r="W46" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -32412,8 +32421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y42" sqref="A1:Y42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.25"/>
@@ -32655,7 +32664,7 @@
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="10">
         <v>21</v>
@@ -32732,7 +32741,7 @@
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="13">
         <v>67</v>
@@ -34259,7 +34268,1582 @@
       <c r="W42" s="6"/>
       <c r="X42" s="6"/>
       <c r="Y42" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:T35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AF13" sqref="AF13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.25"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="20" width="6.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="C1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="D1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="E1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="F1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="G1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="H1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="I1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="J1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="K1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="L1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="M1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="N1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="O1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="P1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="Q1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="R1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="S1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="T1" s="10">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="10">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0</v>
+      </c>
+      <c r="E2" s="10">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10">
+        <v>0</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0</v>
+      </c>
+      <c r="J2" s="10">
+        <v>0</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0</v>
+      </c>
+      <c r="M2" s="10">
+        <v>0</v>
+      </c>
+      <c r="N2" s="10">
+        <v>0</v>
+      </c>
+      <c r="O2" s="10">
+        <v>0</v>
+      </c>
+      <c r="P2" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>0</v>
+      </c>
+      <c r="R2" s="10">
+        <v>0</v>
+      </c>
+      <c r="S2" s="10">
+        <v>0</v>
+      </c>
+      <c r="T2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="S3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="T3" s="10">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="10">
+        <v>6</v>
+      </c>
+      <c r="C4" s="10">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10">
+        <v>6</v>
+      </c>
+      <c r="E4" s="10">
+        <v>14</v>
+      </c>
+      <c r="F4" s="10">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10">
+        <v>14</v>
+      </c>
+      <c r="H4" s="10">
+        <v>21</v>
+      </c>
+      <c r="I4" s="10">
+        <v>21</v>
+      </c>
+      <c r="J4" s="10">
+        <v>21</v>
+      </c>
+      <c r="K4" s="10">
+        <v>28</v>
+      </c>
+      <c r="L4" s="10">
+        <v>28</v>
+      </c>
+      <c r="M4" s="10">
+        <v>28</v>
+      </c>
+      <c r="N4" s="10">
+        <v>35</v>
+      </c>
+      <c r="O4" s="10">
+        <v>35</v>
+      </c>
+      <c r="P4" s="10">
+        <v>35</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>42</v>
+      </c>
+      <c r="R4" s="10">
+        <v>42</v>
+      </c>
+      <c r="S4" s="10">
+        <v>49</v>
+      </c>
+      <c r="T4" s="10">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="13">
+        <v>0</v>
+      </c>
+      <c r="C5" s="13">
+        <v>20</v>
+      </c>
+      <c r="D5" s="13">
+        <v>40</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="13">
+        <v>20</v>
+      </c>
+      <c r="G5" s="13">
+        <v>40</v>
+      </c>
+      <c r="H5" s="13">
+        <v>0</v>
+      </c>
+      <c r="I5" s="13">
+        <v>20</v>
+      </c>
+      <c r="J5" s="13">
+        <v>40</v>
+      </c>
+      <c r="K5" s="13">
+        <v>0</v>
+      </c>
+      <c r="L5" s="13">
+        <v>20</v>
+      </c>
+      <c r="M5" s="13">
+        <v>40</v>
+      </c>
+      <c r="N5" s="13">
+        <v>0</v>
+      </c>
+      <c r="O5" s="13">
+        <v>20</v>
+      </c>
+      <c r="P5" s="13">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="13">
+        <v>0</v>
+      </c>
+      <c r="R5" s="13">
+        <v>20</v>
+      </c>
+      <c r="S5" s="13">
+        <v>0</v>
+      </c>
+      <c r="T5" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>124</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>115</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <v>107</v>
+      </c>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>73</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="1">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1">
+        <v>93</v>
+      </c>
+      <c r="C9" s="1">
+        <v>63</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>65</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1">
+        <v>50</v>
+      </c>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="2">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <v>81</v>
+      </c>
+      <c r="C10" s="2">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2">
+        <v>58</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2">
+        <v>45.5</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2">
+        <v>37</v>
+      </c>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="2"/>
+      <c r="S10" s="2"/>
+      <c r="T10" s="2"/>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="2">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>73</v>
+      </c>
+      <c r="C11" s="2">
+        <v>53</v>
+      </c>
+      <c r="D11" s="2">
+        <v>38.5</v>
+      </c>
+      <c r="E11" s="2">
+        <v>52</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2">
+        <v>41</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2">
+        <v>33.5</v>
+      </c>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2">
+        <v>28.1</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="2"/>
+      <c r="S11" s="2"/>
+      <c r="T11" s="2"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" s="1">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1">
+        <v>49.5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>36.5</v>
+      </c>
+      <c r="E12" s="1">
+        <v>45.5</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1">
+        <v>37.5</v>
+      </c>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1">
+        <v>31</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1">
+        <v>25.9</v>
+      </c>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1">
+        <v>22.4</v>
+      </c>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:20">
+      <c r="A13" s="1">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>62</v>
+      </c>
+      <c r="C13" s="1">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1">
+        <v>35</v>
+      </c>
+      <c r="E13" s="1">
+        <v>41</v>
+      </c>
+      <c r="F13" s="1">
+        <v>29.5</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1">
+        <v>34</v>
+      </c>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1">
+        <v>24</v>
+      </c>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1">
+        <v>20.7</v>
+      </c>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1">
+        <v>17</v>
+      </c>
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="2">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2">
+        <v>52</v>
+      </c>
+      <c r="C14" s="2">
+        <v>41</v>
+      </c>
+      <c r="D14" s="2">
+        <v>32.5</v>
+      </c>
+      <c r="E14" s="2">
+        <v>35.5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>25.9</v>
+      </c>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2">
+        <v>28.2</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="2">
+        <v>24</v>
+      </c>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2">
+        <v>20.7</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2">
+        <v>18</v>
+      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="2">
+        <v>14.8</v>
+      </c>
+      <c r="T14" s="2">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>44.5</v>
+      </c>
+      <c r="C15" s="2">
+        <v>37</v>
+      </c>
+      <c r="D15" s="2">
+        <v>30</v>
+      </c>
+      <c r="E15" s="2">
+        <v>31</v>
+      </c>
+      <c r="F15" s="2">
+        <v>23</v>
+      </c>
+      <c r="G15" s="2">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="H15" s="2">
+        <v>24.7</v>
+      </c>
+      <c r="I15" s="2">
+        <v>18.5</v>
+      </c>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2">
+        <v>20.8</v>
+      </c>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2">
+        <v>17.899999999999999</v>
+      </c>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2">
+        <v>15.8</v>
+      </c>
+      <c r="R15" s="2"/>
+      <c r="S15" s="2">
+        <v>13.1</v>
+      </c>
+      <c r="T15" s="2">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="1">
+        <v>16</v>
+      </c>
+      <c r="B16" s="1">
+        <v>38</v>
+      </c>
+      <c r="C16" s="1">
+        <v>33</v>
+      </c>
+      <c r="D16" s="1">
+        <v>28.3</v>
+      </c>
+      <c r="E16" s="1">
+        <v>26.8</v>
+      </c>
+      <c r="F16" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="G16" s="1">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="H16" s="1">
+        <v>21.8</v>
+      </c>
+      <c r="I16" s="1">
+        <v>16.5</v>
+      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1">
+        <v>18.3</v>
+      </c>
+      <c r="L16" s="1">
+        <v>13.6</v>
+      </c>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1">
+        <v>15.6</v>
+      </c>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1">
+        <v>13.9</v>
+      </c>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="T16" s="1">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
+      <c r="A17" s="1">
+        <v>18</v>
+      </c>
+      <c r="B17" s="1">
+        <v>34</v>
+      </c>
+      <c r="C17" s="1">
+        <v>30.5</v>
+      </c>
+      <c r="D17" s="1">
+        <v>27.1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>23.2</v>
+      </c>
+      <c r="F17" s="1">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="G17" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="H17" s="1">
+        <v>19.3</v>
+      </c>
+      <c r="I17" s="1">
+        <v>14.8</v>
+      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1">
+        <v>16.3</v>
+      </c>
+      <c r="L17" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1">
+        <v>14</v>
+      </c>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1">
+        <v>12.2</v>
+      </c>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="T17" s="1">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
+      <c r="A18" s="2">
+        <v>20</v>
+      </c>
+      <c r="B18" s="2">
+        <v>30.5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>28.7</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="F18" s="2">
+        <v>17.2</v>
+      </c>
+      <c r="G18" s="2">
+        <v>15.2</v>
+      </c>
+      <c r="H18" s="2">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="I18" s="2">
+        <v>13.5</v>
+      </c>
+      <c r="J18" s="2">
+        <v>11.7</v>
+      </c>
+      <c r="K18" s="2">
+        <v>14.6</v>
+      </c>
+      <c r="L18" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2">
+        <v>12.6</v>
+      </c>
+      <c r="O18" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2">
+        <v>11</v>
+      </c>
+      <c r="R18" s="2"/>
+      <c r="S18" s="2">
+        <v>9</v>
+      </c>
+      <c r="T18" s="2">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
+      <c r="A19" s="2">
         <v>22</v>
+      </c>
+      <c r="B19" s="2">
+        <v>27.8</v>
+      </c>
+      <c r="C19" s="2">
+        <v>27.2</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2">
+        <v>17.7</v>
+      </c>
+      <c r="F19" s="2">
+        <v>15.7</v>
+      </c>
+      <c r="G19" s="2">
+        <v>14.3</v>
+      </c>
+      <c r="H19" s="2">
+        <v>15</v>
+      </c>
+      <c r="I19" s="2">
+        <v>12.3</v>
+      </c>
+      <c r="J19" s="2">
+        <v>10.8</v>
+      </c>
+      <c r="K19" s="2">
+        <v>13</v>
+      </c>
+      <c r="L19" s="2">
+        <v>9.9</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2">
+        <v>11.4</v>
+      </c>
+      <c r="O19" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2">
+        <v>10</v>
+      </c>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2">
+        <v>8.1</v>
+      </c>
+      <c r="T19" s="2">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
+      <c r="A20" s="1">
+        <v>24</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="F20" s="1">
+        <v>14.5</v>
+      </c>
+      <c r="G20" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="H20" s="1">
+        <v>13.1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>11.3</v>
+      </c>
+      <c r="J20" s="1">
+        <v>10</v>
+      </c>
+      <c r="K20" s="1">
+        <v>11.6</v>
+      </c>
+      <c r="L20" s="1">
+        <v>9</v>
+      </c>
+      <c r="M20" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="N20" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="O20" s="1">
+        <v>8</v>
+      </c>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="R20" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="S20" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="T20" s="1">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
+      <c r="A21" s="1">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1">
+        <v>14.6</v>
+      </c>
+      <c r="F21" s="1">
+        <v>13.5</v>
+      </c>
+      <c r="G21" s="1">
+        <v>13</v>
+      </c>
+      <c r="H21" s="1">
+        <v>11.5</v>
+      </c>
+      <c r="I21" s="1">
+        <v>10.4</v>
+      </c>
+      <c r="J21" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="K21" s="1">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="L21" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="M21" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="N21" s="1">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="O21" s="1">
+        <v>7.2</v>
+      </c>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="R21" s="1">
+        <v>6.2</v>
+      </c>
+      <c r="S21" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="T21" s="1">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="2">
+        <v>28</v>
+      </c>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2">
+        <v>13.4</v>
+      </c>
+      <c r="F22" s="2">
+        <v>12.9</v>
+      </c>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="I22" s="2">
+        <v>9.5</v>
+      </c>
+      <c r="J22" s="2">
+        <v>8.9</v>
+      </c>
+      <c r="K22" s="2">
+        <v>9</v>
+      </c>
+      <c r="L22" s="2">
+        <v>7.6</v>
+      </c>
+      <c r="M22" s="2">
+        <v>6.6</v>
+      </c>
+      <c r="N22" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="O22" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="R22" s="2">
+        <v>5.6</v>
+      </c>
+      <c r="S22" s="2">
+        <v>6.1</v>
+      </c>
+      <c r="T22" s="2">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="2">
+        <v>30</v>
+      </c>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2">
+        <v>12.4</v>
+      </c>
+      <c r="F23" s="2">
+        <v>12.3</v>
+      </c>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2">
+        <v>9.6</v>
+      </c>
+      <c r="I23" s="2">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="J23" s="2">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="K23" s="2">
+        <v>7.9</v>
+      </c>
+      <c r="L23" s="2">
+        <v>7</v>
+      </c>
+      <c r="M23" s="2">
+        <v>6.2</v>
+      </c>
+      <c r="N23" s="2">
+        <v>7.3</v>
+      </c>
+      <c r="O23" s="2">
+        <v>6</v>
+      </c>
+      <c r="P23" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>6.8</v>
+      </c>
+      <c r="R23" s="2">
+        <v>5</v>
+      </c>
+      <c r="S23" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="T23" s="2">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
+      <c r="A24" s="1">
+        <v>32</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I24" s="1">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J24" s="1">
+        <v>8</v>
+      </c>
+      <c r="K24" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="L24" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="M24" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="N24" s="1">
+        <v>6.4</v>
+      </c>
+      <c r="O24" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="P24" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="Q24" s="1">
+        <v>6.1</v>
+      </c>
+      <c r="R24" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="S24" s="1">
+        <v>5</v>
+      </c>
+      <c r="T24" s="1">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
+      <c r="A25" s="1">
+        <v>34</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="I25" s="1">
+        <v>7.8</v>
+      </c>
+      <c r="J25" s="1">
+        <v>7.7</v>
+      </c>
+      <c r="K25" s="1">
+        <v>6.5</v>
+      </c>
+      <c r="L25" s="1">
+        <v>5.8</v>
+      </c>
+      <c r="M25" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="N25" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="O25" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="P25" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="Q25" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="R25" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="S25" s="1">
+        <v>4.5</v>
+      </c>
+      <c r="T25" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
+      <c r="A26" s="2">
+        <v>36</v>
+      </c>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="I26" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="J26" s="2"/>
+      <c r="K26" s="2">
+        <v>6</v>
+      </c>
+      <c r="L26" s="2">
+        <v>5.4</v>
+      </c>
+      <c r="M26" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="N26" s="2">
+        <v>5</v>
+      </c>
+      <c r="O26" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="P26" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="R26" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="S26" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="T26" s="2"/>
+    </row>
+    <row r="27" spans="1:20">
+      <c r="A27" s="2">
+        <v>38</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2">
+        <v>7</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="2">
+        <v>5</v>
+      </c>
+      <c r="L27" s="2">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M27" s="2">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="N27" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="O27" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="P27" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="R27" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="S27" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="T27" s="2"/>
+    </row>
+    <row r="28" spans="1:20">
+      <c r="A28" s="1">
+        <v>40</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1">
+        <v>5</v>
+      </c>
+      <c r="L28" s="1">
+        <v>4.8</v>
+      </c>
+      <c r="M28" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="N28" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="O28" s="1">
+        <v>4</v>
+      </c>
+      <c r="P28" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="R28" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="S28" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="T28" s="1"/>
+    </row>
+    <row r="29" spans="1:20">
+      <c r="A29" s="1">
+        <v>42</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1">
+        <v>4.7</v>
+      </c>
+      <c r="L29" s="1">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1">
+        <v>3.9</v>
+      </c>
+      <c r="O29" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="P29" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>3.3</v>
+      </c>
+      <c r="R29" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+    </row>
+    <row r="30" spans="1:20">
+      <c r="A30" s="2">
+        <v>44</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L30" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="O30" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="P30" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="R30" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="S30" s="2"/>
+      <c r="T30" s="2"/>
+    </row>
+    <row r="31" spans="1:20">
+      <c r="A31" s="2">
+        <v>46</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="O31" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="P31" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="R31" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="S31" s="2"/>
+      <c r="T31" s="2"/>
+    </row>
+    <row r="32" spans="1:20">
+      <c r="A32" s="1">
+        <v>48</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="O32" s="1">
+        <v>3.1</v>
+      </c>
+      <c r="P32" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>2.6</v>
+      </c>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+    </row>
+    <row r="33" spans="1:20">
+      <c r="A33" s="1">
+        <v>50</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="O33" s="1">
+        <v>2.9</v>
+      </c>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+    </row>
+    <row r="34" spans="1:20">
+      <c r="A34" s="2">
+        <v>52</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+    </row>
+    <row r="35" spans="1:20">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -34273,7 +35857,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:J5"/>
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25"/>
@@ -36651,7 +38235,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I5"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25"/>
@@ -37362,7 +38946,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -37376,7 +38960,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I5"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25"/>
@@ -38107,7 +39691,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="6" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -38120,8 +39704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA54"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:AA5"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AB50" sqref="AB50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25"/>
@@ -40629,7 +42213,7 @@
   <dimension ref="A1:F51"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D5" sqref="A1:D5"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="17.25"/>

</xml_diff>